<commit_message>
added images for 404 error, changes background
</commit_message>
<xml_diff>
--- a/CODE_WOOKIE/uploading_Bash_Script/orderlist.xlsx
+++ b/CODE_WOOKIE/uploading_Bash_Script/orderlist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>01--02</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>PLAN_DEC2013_JAN2014_ONLY</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,8 +630,11 @@
       <c r="C10" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
       <c r="F10" s="6">
-        <v>49525</v>
+        <v>16118</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
@@ -649,9 +655,16 @@
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="6">
+        <f>49525-17058-16118</f>
+        <v>16349</v>
+      </c>
       <c r="G11" s="1">
-        <f t="shared" si="0"/>
-        <v>194445</v>
+        <f>G10+F10</f>
+        <v>161038</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -668,9 +681,15 @@
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="6">
+        <v>17058</v>
+      </c>
       <c r="G12" s="1">
-        <f t="shared" si="0"/>
-        <v>194445</v>
+        <f>G11+F11</f>
+        <v>177387</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -688,8 +707,8 @@
         <v>9</v>
       </c>
       <c r="F13">
-        <f>51590-17687</f>
-        <v>33903</v>
+        <f>51590-17687-17232</f>
+        <v>16671</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
@@ -710,9 +729,12 @@
       <c r="C14" s="3">
         <v>10</v>
       </c>
+      <c r="F14">
+        <v>17232</v>
+      </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>228348</v>
+        <v>211116</v>
       </c>
       <c r="H14">
         <v>7</v>

</xml_diff>